<commit_message>
all notebooks reran with CMap
</commit_message>
<xml_diff>
--- a/Notebooks/results/drugs_to_validate.xlsx
+++ b/Notebooks/results/drugs_to_validate.xlsx
@@ -25,25 +25,25 @@
     <t>G3</t>
   </si>
   <si>
-    <t>mean_score(G3)</t>
+    <t>mean_rank(G3)</t>
   </si>
   <si>
     <t>G4</t>
   </si>
   <si>
-    <t>mean_score(G4)</t>
+    <t>mean_rank(G4)</t>
   </si>
   <si>
     <t>SHH</t>
   </si>
   <si>
-    <t>mean_score(SHH)</t>
+    <t>mean_rank(SHH)</t>
   </si>
   <si>
     <t>SHH+p53</t>
   </si>
   <si>
-    <t>mean_score(SHH+p53)</t>
+    <t>mean_rank(SHH+p53)</t>
   </si>
   <si>
     <t>SBI</t>
@@ -55,39 +55,39 @@
     <t>gsk1070916</t>
   </si>
   <si>
+    <t>bx-912</t>
+  </si>
+  <si>
+    <t>abt-737</t>
+  </si>
+  <si>
     <t>linsitinib</t>
   </si>
   <si>
-    <t>bx-912</t>
-  </si>
-  <si>
-    <t>abt-737</t>
-  </si>
-  <si>
     <t>['SBI-0654453.P001']</t>
   </si>
   <si>
+    <t>['SBI-0645949.P001']</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
     <t>['SBI-0646932.P001']</t>
   </si>
   <si>
-    <t>['SBI-0645949.P001']</t>
-  </si>
-  <si>
-    <t>[]</t>
-  </si>
-  <si>
     <t>SBI-0654453.P001</t>
   </si>
   <si>
+    <t>SBI-0645949.P001</t>
+  </si>
+  <si>
+    <t>NaN</t>
+  </si>
+  <si>
     <t>SBI-0646932.P001</t>
   </si>
   <si>
-    <t>SBI-0645949.P001</t>
-  </si>
-  <si>
-    <t>NaN</t>
-  </si>
-  <si>
     <t>etoposide</t>
   </si>
   <si>
@@ -124,10 +124,10 @@
     <t>SBI-0646927.P001</t>
   </si>
   <si>
+    <t>olaparib</t>
+  </si>
+  <si>
     <t>rucaparib</t>
-  </si>
-  <si>
-    <t>olaparib</t>
   </si>
 </sst>
 </file>
@@ -528,7 +528,7 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -537,25 +537,25 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>0.6399999999999999</v>
+        <v>2.1</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="F2">
-        <v>0.6435</v>
+        <v>2.75</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>0.6110000000000001</v>
+        <v>2</v>
       </c>
       <c r="I2">
         <v>1</v>
       </c>
       <c r="J2">
-        <v>0.6136666666666667</v>
+        <v>2</v>
       </c>
       <c r="K2" t="s">
         <v>15</v>
@@ -566,7 +566,7 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="1">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
@@ -575,25 +575,25 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>0.5565</v>
+        <v>10.4</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="F3">
-        <v>0.5585</v>
+        <v>8.75</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>0.528</v>
+        <v>116</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3">
-        <v>0.5343333333333334</v>
+        <v>223</v>
       </c>
       <c r="K3" t="s">
         <v>16</v>
@@ -604,7 +604,7 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="1">
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
@@ -613,25 +613,25 @@
         <v>1</v>
       </c>
       <c r="D4">
-        <v>0.5365999999999999</v>
+        <v>32.05</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4">
-        <v>0.5412500000000001</v>
+        <v>32.75</v>
       </c>
       <c r="G4">
         <v>1</v>
       </c>
       <c r="H4">
-        <v>0.3376666666666666</v>
+        <v>33.41666666666666</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4">
-        <v>0.1813333333333333</v>
+        <v>33.83333333333334</v>
       </c>
       <c r="K4" t="s">
         <v>17</v>
@@ -642,7 +642,7 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="1">
-        <v>27</v>
+        <v>108</v>
       </c>
       <c r="B5" t="s">
         <v>14</v>
@@ -651,25 +651,25 @@
         <v>1</v>
       </c>
       <c r="D5">
-        <v>0.4227</v>
+        <v>84.34999999999999</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5">
-        <v>0.41675</v>
+        <v>88.75</v>
       </c>
       <c r="G5">
         <v>1</v>
       </c>
       <c r="H5">
-        <v>0.3966666666666667</v>
+        <v>87.25</v>
       </c>
       <c r="I5">
         <v>1</v>
       </c>
       <c r="J5">
-        <v>0.408</v>
+        <v>86.5</v>
       </c>
       <c r="K5" t="s">
         <v>18</v>
@@ -728,7 +728,7 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="1">
-        <v>221</v>
+        <v>135</v>
       </c>
       <c r="B2" t="s">
         <v>23</v>
@@ -737,25 +737,25 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0.2413</v>
+        <v>156.95</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>0.15525</v>
+        <v>167.625</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2">
-        <v>0.1475</v>
+        <v>163.5</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
       <c r="J2">
-        <v>0.04900000000000001</v>
+        <v>184.6666666666667</v>
       </c>
       <c r="K2" t="s">
         <v>25</v>
@@ -766,7 +766,7 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="1">
-        <v>223</v>
+        <v>149</v>
       </c>
       <c r="B3" t="s">
         <v>24</v>
@@ -775,25 +775,25 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>0.2718</v>
+        <v>228.05</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>0.166</v>
+        <v>217.25</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3">
-        <v>0.07266666666666667</v>
+        <v>214.6666666666667</v>
       </c>
       <c r="I3">
         <v>0</v>
       </c>
       <c r="J3">
-        <v>0.1093333333333333</v>
+        <v>189</v>
       </c>
       <c r="K3" t="s">
         <v>26</v>
@@ -852,7 +852,7 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="1">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
         <v>29</v>
@@ -861,25 +861,25 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>0.5614</v>
+        <v>7.9</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="F2">
-        <v>0.5467500000000001</v>
+        <v>8.5</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>0.5193333333333333</v>
+        <v>7.666666666666667</v>
       </c>
       <c r="I2">
         <v>1</v>
       </c>
       <c r="J2">
-        <v>0.5276666666666667</v>
+        <v>7</v>
       </c>
       <c r="K2" t="s">
         <v>31</v>
@@ -890,7 +890,7 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="1">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
         <v>30</v>
@@ -899,25 +899,25 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>0.3872</v>
+        <v>34.3</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="F3">
-        <v>0.34575</v>
+        <v>48.25</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>0.3373333333333333</v>
+        <v>55.25</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>0.3636666666666666</v>
+        <v>42.5</v>
       </c>
       <c r="K3" t="s">
         <v>32</v>
@@ -976,7 +976,7 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="1">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
         <v>35</v>
@@ -985,36 +985,36 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0.2085</v>
+        <v>155.9</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>0.50925</v>
+        <v>113.75</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>0.4929999999999999</v>
+        <v>23</v>
       </c>
       <c r="I2">
         <v>1</v>
       </c>
       <c r="J2">
-        <v>0.4986666666666666</v>
+        <v>22.83333333333333</v>
       </c>
       <c r="K2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="1">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
         <v>36</v>
@@ -1023,31 +1023,31 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>0.1674</v>
+        <v>113.4</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3">
-        <v>0.18825</v>
+        <v>21.75</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>0.3965</v>
+        <v>15.75</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>0.4116666666666666</v>
+        <v>16.16666666666667</v>
       </c>
       <c r="K3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
backup on 2019-04-18, before preparing for publication
</commit_message>
<xml_diff>
--- a/Notebooks/results/drugs_to_validate.xlsx
+++ b/Notebooks/results/drugs_to_validate.xlsx
@@ -1,23 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10123"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edjuaro/GoogleDrive/pdx/pdx-hts/Notebooks/results/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D87F9B2C-B465-1C42-BF63-8B6A2ED3C749}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="760" yWindow="460" windowWidth="18820" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="G3_effective" sheetId="1" r:id="rId1"/>
-    <sheet name="G3_ineffective" sheetId="2" r:id="rId2"/>
-    <sheet name="notG3_effective" sheetId="3" r:id="rId3"/>
-    <sheet name="SHH_effective" sheetId="4" r:id="rId4"/>
+    <sheet name="all" sheetId="6" r:id="rId1"/>
+    <sheet name="G3_effective" sheetId="1" r:id="rId2"/>
+    <sheet name="G3_ineffective" sheetId="2" r:id="rId3"/>
+    <sheet name="notG3_effective" sheetId="3" r:id="rId4"/>
+    <sheet name="SHH_effective" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="38">
   <si>
     <t>Name</t>
   </si>
@@ -128,13 +142,16 @@
   </si>
   <si>
     <t>rucaparib</t>
+  </si>
+  <si>
+    <t>index</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -197,6 +214,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -243,7 +268,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -275,9 +300,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -309,6 +352,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -484,14 +545,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EE18100-3C1D-C140-AFE6-14D9889A98EE}">
+  <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -526,7 +592,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>4</v>
       </c>
@@ -564,7 +630,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>11</v>
       </c>
@@ -602,7 +668,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>44</v>
       </c>
@@ -613,7 +679,7 @@
         <v>1</v>
       </c>
       <c r="D4">
-        <v>32.05</v>
+        <v>32.049999999999997</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -625,13 +691,13 @@
         <v>1</v>
       </c>
       <c r="H4">
-        <v>33.41666666666666</v>
+        <v>33.416666666666657</v>
       </c>
       <c r="I4">
         <v>1</v>
       </c>
       <c r="J4">
-        <v>33.83333333333334</v>
+        <v>33.833333333333343</v>
       </c>
       <c r="K4" t="s">
         <v>17</v>
@@ -640,7 +706,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>108</v>
       </c>
@@ -651,7 +717,7 @@
         <v>1</v>
       </c>
       <c r="D5">
-        <v>84.34999999999999</v>
+        <v>84.35</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -676,6 +742,234 @@
       </c>
       <c r="L5" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>135</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>156.94999999999999</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>167.625</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>163.5</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>184.66666666666671</v>
+      </c>
+      <c r="K6" t="s">
+        <v>25</v>
+      </c>
+      <c r="L6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>149</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>228.05</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>217.25</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>214.66666666666671</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>189</v>
+      </c>
+      <c r="K7" t="s">
+        <v>26</v>
+      </c>
+      <c r="L7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>7.9</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>8.5</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>7.666666666666667</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>7</v>
+      </c>
+      <c r="K8" t="s">
+        <v>31</v>
+      </c>
+      <c r="L8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>64</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>34.299999999999997</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>48.25</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>55.25</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>42.5</v>
+      </c>
+      <c r="K9" t="s">
+        <v>32</v>
+      </c>
+      <c r="L9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>155.9</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>113.75</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>23</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>22.833333333333329</v>
+      </c>
+      <c r="K10" t="s">
+        <v>17</v>
+      </c>
+      <c r="L10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>40</v>
+      </c>
+      <c r="B11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>113.4</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>21.75</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>15.75</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>16.166666666666671</v>
+      </c>
+      <c r="K11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L11" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -684,14 +978,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:L5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -726,80 +1022,156 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>135</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>156.95</v>
+        <v>2.1</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2">
-        <v>167.625</v>
+        <v>2.75</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2">
-        <v>163.5</v>
+        <v>2</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2">
-        <v>184.6666666666667</v>
+        <v>2</v>
       </c>
       <c r="K2" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="L2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>149</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>228.05</v>
+        <v>10.4</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3">
-        <v>217.25</v>
+        <v>8.75</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3">
-        <v>214.6666666666667</v>
+        <v>116</v>
       </c>
       <c r="I3">
         <v>0</v>
       </c>
       <c r="J3">
-        <v>189</v>
+        <v>223</v>
       </c>
       <c r="K3" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="L3" t="s">
-        <v>28</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>44</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>32.049999999999997</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>32.75</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>33.416666666666657</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>33.833333333333343</v>
+      </c>
+      <c r="K4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>108</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>84.35</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>88.75</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>87.25</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>86.5</v>
+      </c>
+      <c r="K5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -808,14 +1180,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:L3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -850,80 +1224,80 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>12</v>
+        <v>135</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>7.9</v>
+        <v>156.94999999999999</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>8.5</v>
+        <v>167.625</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>7.666666666666667</v>
+        <v>163.5</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2">
-        <v>7</v>
+        <v>184.66666666666671</v>
       </c>
       <c r="K2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="L2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>64</v>
+        <v>149</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>34.3</v>
+        <v>228.05</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>48.25</v>
+        <v>217.25</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>55.25</v>
+        <v>214.66666666666671</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3">
-        <v>42.5</v>
+        <v>189</v>
       </c>
       <c r="K3" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="L3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -932,14 +1306,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:L3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -974,7 +1350,133 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>7.9</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>8.5</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>7.666666666666667</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>7</v>
+      </c>
+      <c r="K2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>64</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>34.299999999999997</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>48.25</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>55.25</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>42.5</v>
+      </c>
+      <c r="K3" t="s">
+        <v>32</v>
+      </c>
+      <c r="L3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:L3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:L3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>35</v>
       </c>
@@ -1003,7 +1505,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>22.83333333333333</v>
+        <v>22.833333333333329</v>
       </c>
       <c r="K2" t="s">
         <v>17</v>
@@ -1012,7 +1514,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>40</v>
       </c>
@@ -1041,7 +1543,7 @@
         <v>1</v>
       </c>
       <c r="J3">
-        <v>16.16666666666667</v>
+        <v>16.166666666666671</v>
       </c>
       <c r="K3" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
step_5 updated and reran
</commit_message>
<xml_diff>
--- a/Notebooks/results/drugs_to_validate.xlsx
+++ b/Notebooks/results/drugs_to_validate.xlsx
@@ -11,13 +11,15 @@
     <sheet name="G3_ineffective" sheetId="2" r:id="rId2"/>
     <sheet name="notG3_effective" sheetId="3" r:id="rId3"/>
     <sheet name="SHH_effective" sheetId="4" r:id="rId4"/>
+    <sheet name="all_drugs_present" sheetId="5" r:id="rId5"/>
+    <sheet name="not_in_DiSCoVER" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="40">
   <si>
     <t>Name</t>
   </si>
@@ -128,6 +130,15 @@
   </si>
   <si>
     <t>olaparib</t>
+  </si>
+  <si>
+    <t>not_found</t>
+  </si>
+  <si>
+    <t>anisomycin</t>
+  </si>
+  <si>
+    <t>monafide</t>
   </si>
 </sst>
 </file>
@@ -1053,4 +1064,466 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0.6399999999999999</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>0.6435</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>0.611</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>0.6136666666666667</v>
+      </c>
+      <c r="K2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="1">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0.5614</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>0.5467500000000001</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>0.5193333333333333</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>0.5276666666666667</v>
+      </c>
+      <c r="K3" t="s">
+        <v>31</v>
+      </c>
+      <c r="L3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="1">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>0.5565</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>0.5585</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>0.528</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>0.5343333333333334</v>
+      </c>
+      <c r="K4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="1">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0.5365999999999999</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>0.5412500000000001</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>0.3376666666666666</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0.1813333333333333</v>
+      </c>
+      <c r="K5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="1">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0.2085</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>0.50925</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>0.4929999999999999</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>0.4986666666666666</v>
+      </c>
+      <c r="K6" t="s">
+        <v>18</v>
+      </c>
+      <c r="L6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="1">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0.4227</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>0.41675</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>0.3966666666666667</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>0.408</v>
+      </c>
+      <c r="K7" t="s">
+        <v>18</v>
+      </c>
+      <c r="L7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="1">
+        <v>37</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>0.3872</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>0.34575</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>0.3373333333333333</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>0.3636666666666666</v>
+      </c>
+      <c r="K8" t="s">
+        <v>32</v>
+      </c>
+      <c r="L8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="1">
+        <v>38</v>
+      </c>
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0.1674</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0.18825</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>0.3965</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>0.4116666666666666</v>
+      </c>
+      <c r="K9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="1">
+        <v>89</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0.2413</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0.15525</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0.1475</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0.04900000000000001</v>
+      </c>
+      <c r="K10" t="s">
+        <v>25</v>
+      </c>
+      <c r="L10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="1">
+        <v>158</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0.2718</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0.166</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0.07266666666666667</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0.1093333333333333</v>
+      </c>
+      <c r="K11" t="s">
+        <v>26</v>
+      </c>
+      <c r="L11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="B1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>